<commit_message>
vault backup: 2025-05-26 11:56:38
</commit_message>
<xml_diff>
--- a/Chemistry/Year 12/Assignments/IA2/Results/Chemistry experiment data IA2.xlsx
+++ b/Chemistry/Year 12/Assignments/IA2/Results/Chemistry experiment data IA2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gc021263\Obsidian\NoahsObsidianSync\Chemistry\Year 12\Assignments\IA2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4346EEC7-8CAA-4DDA-8C28-E5E537A40F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A0A101-6B5B-4E98-8635-74901DE335A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{C5BF1A31-5F8B-4741-AA60-1E2AB135D676}"/>
   </bookViews>
@@ -16,6 +16,12 @@
     <sheet name="Raw data IA2" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet2!$A$3:$A$10</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet2!$B$3:$B$10</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet2!$A$3:$A$10</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet2!$B$3:$B$10</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Calculation prep</t>
   </si>
@@ -76,6 +82,12 @@
   </si>
   <si>
     <t>Average voltage (V)</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>Trial 1</t>
   </si>
 </sst>
 </file>
@@ -779,18 +791,37 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.7152411398412872E-2"/>
+          <c:y val="0.1670646058947497"/>
+          <c:w val="0.74009022253418799"/>
+          <c:h val="0.72880370672233563"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Trial 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -810,6 +841,58 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.10383625770388795"/>
+                  <c:y val="-5.4526293753538582E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet2!$A$3:$A$10</c:f>
@@ -876,10 +959,173 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D302-4E64-B637-44E4C99DA3CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.8318115497489521E-2"/>
+                  <c:y val="0.18812701141964996"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$3:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.68066666666666664</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.49466666666666664</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4306666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48133333333333334</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.44800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.44133333333333336</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-02DB-4143-97EA-FE563EAE41DE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1026,6 +1272,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2227,16 +2504,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>539994</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>123581</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>326570</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>18143</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2923,10 +3200,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D75EC8-0243-465F-A593-A949321AC039}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="105" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2934,7 +3211,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2946,10 +3223,13 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -2958,7 +3238,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2975,8 +3255,12 @@
         <f>AVERAGE(B3:D3)</f>
         <v>0.68066666666666664</v>
       </c>
+      <c r="F3">
+        <f>(MAX(B3:D3)-MIN(B3:D3))*0.5</f>
+        <v>2.0999999999999963E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.85</v>
       </c>
@@ -2993,8 +3277,12 @@
         <f t="shared" ref="E4:E10" si="0">AVERAGE(B4:D4)</f>
         <v>0.59166666666666667</v>
       </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F10" si="1">(MAX(B4:D4)-MIN(B4:D4))*0.5</f>
+        <v>8.8000000000000023E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.7</v>
       </c>
@@ -3011,8 +3299,12 @@
         <f t="shared" si="0"/>
         <v>0.49466666666666664</v>
       </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>5.1000000000000018E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.55000000000000004</v>
       </c>
@@ -3029,8 +3321,12 @@
         <f t="shared" si="0"/>
         <v>0.4306666666666667</v>
       </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>2.200000000000002E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.4</v>
       </c>
@@ -3047,8 +3343,12 @@
         <f t="shared" si="0"/>
         <v>0.42199999999999999</v>
       </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>1.3000000000000012E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.3</v>
       </c>
@@ -3065,8 +3365,12 @@
         <f t="shared" si="0"/>
         <v>0.48133333333333334</v>
       </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>1.4000000000000012E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.2</v>
       </c>
@@ -3083,8 +3387,12 @@
         <f t="shared" si="0"/>
         <v>0.44800000000000001</v>
       </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>4.3999999999999984E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.1</v>
       </c>
@@ -3101,8 +3409,12 @@
         <f t="shared" si="0"/>
         <v>0.44133333333333336</v>
       </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>2.8999999999999998E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3110,7 +3422,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -3119,30 +3431,30 @@
         <v>0.68066666666666664</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.85</v>
       </c>
       <c r="B14">
-        <f t="shared" ref="B14:B20" si="1">E4</f>
+        <f t="shared" ref="B14:B20" si="2">E4</f>
         <v>0.59166666666666667</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.7</v>
       </c>
       <c r="B15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.49466666666666664</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.55000000000000004</v>
       </c>
       <c r="B16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.4306666666666667</v>
       </c>
     </row>
@@ -3151,7 +3463,7 @@
         <v>0.4</v>
       </c>
       <c r="B17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.42199999999999999</v>
       </c>
     </row>
@@ -3160,7 +3472,7 @@
         <v>0.3</v>
       </c>
       <c r="B18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.48133333333333334</v>
       </c>
     </row>
@@ -3169,7 +3481,7 @@
         <v>0.2</v>
       </c>
       <c r="B19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.44800000000000001</v>
       </c>
     </row>
@@ -3178,7 +3490,7 @@
         <v>0.1</v>
       </c>
       <c r="B20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.44133333333333336</v>
       </c>
     </row>

</xml_diff>